<commit_message>
Enforced common elective slots with day separation for all branches & sections
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
@@ -9,6 +9,10 @@
   <sheets>
     <sheet name="Section_A" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Section_B" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Basket_Allocation" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Course_Summary" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Basket_Courses" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Common_Slots_Info" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -469,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>DS161</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>HS161</t>
         </is>
       </c>
     </row>
@@ -501,22 +505,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>HS161</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MA161</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>DS161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -565,7 +569,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -575,17 +579,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>CS161</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Free</t>
         </is>
       </c>
     </row>
@@ -597,7 +601,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1 (Tutorial)</t>
+          <t>EC161 (Tutorial)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -617,7 +621,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -629,27 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>MA161</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>HS161</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>EC161</t>
         </is>
       </c>
     </row>
@@ -661,27 +665,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS161 (Tutorial)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA161 (Tutorial)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162 (Tutorial)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 (Tutorial)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -739,27 +743,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -771,27 +775,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Free</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>MA162</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>MA161</t>
         </is>
       </c>
     </row>
@@ -835,27 +839,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>CS161</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161</t>
         </is>
       </c>
     </row>
@@ -867,7 +871,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Basket: ELECTIVE_B1 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -882,12 +886,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 (Tutorial)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>ELECTIVE_B1 (Tutorial)</t>
         </is>
       </c>
     </row>
@@ -904,22 +908,22 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -931,27 +935,2819 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 (Tutorial)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS161 (Tutorial)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 (Tutorial)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA161 (Tutorial)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162 (Tutorial)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Basket Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture Slot 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture Slot 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorial Slot</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Courses in Basket</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Common for Both Sections</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Days Separation</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Applicable Branches</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Slot Type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>PH151, DS151, CS101, CS151, HS157, HS102, HS103, DE101, HS156, HS152, PH151, DS151, CS101, HS157, HS102, HS103, DE101, HS156, CS161, PH151, DS151, CS101, HS157, HS102, HS103, DE101, HS156, CS161</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>✅ YES</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>✅ YES</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>✅ YES</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSE, DSAI, ECE (ALL)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>FIXED COMMON SLOTS</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Course Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Branch Specificity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>LTPSC</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lectures/Week</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorials/Week</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Total Credits</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Introduction to data science and artifical inteligance</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3-0-2-0-2</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3-0-2-0-4</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Department: CSE</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Introduction to quantam Physics</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Linux for Engineers</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computing</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Kannada Kali-Nali</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Leveraging IT for Better Life</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Basics of Design</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Economics/IET</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>3-0-0-0-3</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Introduction to quantum Physics</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Linux for Engineers</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computing</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Computational Thinking</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Kannada Kali-Nali</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Leveraging IT for Better Life</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Basics of Design</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Introduction to quantum physics</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Linux for Engineers</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Fundamentals of Computing</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Computational musicology for hindustani music</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Kannada Kali-Nali</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>2</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Leveraging IT for Better Life</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Basics of Design</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1-0-0-0-1</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>introduction to cyber security</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Elective</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2-0-0-0-2</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Basket Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture Slots</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorial Slot</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Courses in Basket</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Common for All Branches</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Common for Both Sections</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>28</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>28</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>28</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>28</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>28</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>28</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>28</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>28</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>28</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HS152</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>28</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>28</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>28</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>28</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>28</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>28</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>28</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>28</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>28</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>28</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>28</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>DS151</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>28</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>28</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>28</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>HS102</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>28</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>HS103</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>28</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>DE101</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>28</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>28</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Mon 09:00-10:30, Wed 09:00-10:30</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Fri 14:30-15:30</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>28</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Basket Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture 1 Day</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture 1 Time</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture 2 Day</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lecture 2 Time</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorial Day</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Tutorial Time</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Courses</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Common for Branches</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Common for Sections</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Days Separation</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Slot Consistency</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mon</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>09:00-10:30</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Wed</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>09:00-10:30</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Fri</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>14:30-15:30</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>PH151, DS151, CS101, CS151, HS157, HS102, HS103, DE101, HS156, HS152, PH151, DS151, CS101, HS157, HS102, HS103, DE101, HS156, CS161, PH151, DS151, CS101, HS157, HS102, HS103, DE101, HS156, CS161</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>CSE, DSAI, ECE (ALL)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>A &amp; B (BOTH)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>✅ Achieved</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>✅ IDENTICAL across all</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>FIXED COMMON TIMETABLE SLOTS</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Specific Baskets B6 and B7 for semester 7
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
@@ -13,6 +13,8 @@
     <sheet name="Course_Summary" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Basket_Courses" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Common_Slots_Info" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Semester_Rules" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Classroom_Utilization" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -473,7 +475,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>ELECTIVE_B1 [C405]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,17 +485,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>ELECTIVE_B1 [C405]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 [C405]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>DS161 [C405]</t>
         </is>
       </c>
     </row>
@@ -505,27 +507,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>EC161 [C405]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>CS161 [C405]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>MA161 [C405]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>MA162</t>
         </is>
       </c>
     </row>
@@ -569,27 +571,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>MA161 [C405]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>EC161 [C405]</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>HS161 [C405]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Free</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>EC161</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>CS161</t>
         </is>
       </c>
     </row>
@@ -601,27 +603,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EC161 (Tutorial)</t>
+          <t>EC161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>DS161 (Tutorial) [C405]</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>HS161 (Tutorial) [C405]</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Free</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 (Tutorial)</t>
+          <t>ELECTIVE_B1 (Tutorial) [C405]</t>
         </is>
       </c>
     </row>
@@ -633,27 +635,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>MA162 [C405]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>CS161 [C405]</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>CS161</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>MA162 [C405]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 [C405]</t>
         </is>
       </c>
     </row>
@@ -665,27 +667,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CS161 (Tutorial)</t>
+          <t>CS161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MA161 (Tutorial)</t>
+          <t>MA162 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MA162 (Tutorial)</t>
+          <t>MA161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>DS161 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>HS161 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -743,27 +745,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>ELECTIVE_B1 [C405]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>ELECTIVE_B1 [C405]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>MA162 [C405]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS161 [C405]</t>
         </is>
       </c>
     </row>
@@ -775,27 +777,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS161 [C405]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>MA161 [C405]</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Free</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MA162</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>CS161 [C405]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>EC161 [C405]</t>
         </is>
       </c>
     </row>
@@ -844,22 +846,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>MA162 [C405]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -871,27 +873,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>CS161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>DS161 (Tutorial)</t>
+          <t>MA161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 (Tutorial)</t>
+          <t>ELECTIVE_B1 (Tutorial) [C405]</t>
         </is>
       </c>
     </row>
@@ -903,27 +905,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>EC161 [C405]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 [C405]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>MA161 [C405]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 [C405]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 [C405]</t>
         </is>
       </c>
     </row>
@@ -935,27 +937,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>HS161 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CS161 (Tutorial)</t>
+          <t>EC161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>EC161 (Tutorial)</t>
+          <t>HS161 (Tutorial) [C405]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>MA161 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>MA162 (Tutorial)</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -3754,4 +3756,1334 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Rule</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exclusion</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Scheduled Baskets</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Semester 1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Schedule all elective baskets</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>No specific restrictions for this semester</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ELECTIVE_B1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>✅ Applied</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Room Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Capacity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Weekly Hours (Timetable)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Daily Avg Hours (Timetable)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Exam Sessions</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Utilization Rate (%)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Facilities</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Recreation</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>large classroom</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>116</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>large classroom</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Auditorium</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C101</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C102</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>C103</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>library</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>C104</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>L105</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Hardware Lab</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Hardware Equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>L106</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Software Lab</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>L107</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Software Lab</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C201</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C202</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>C203</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C204</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C205</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>L206</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Hardware Lab</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Hardware Equipment</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>L207</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Software Lab</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>L208</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Software Lab</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C301</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Physics Lab</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C302</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C303</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C304</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C305</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>L306</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>L307</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Research Scholar Lab</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>L308</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Research Scholar Lab</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C401</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C402</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C403</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>C404</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>C405</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>56</v>
+      </c>
+      <c r="E33" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>100</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>L406</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>L407</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>L408</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>classroom without projector</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
separate pre mid and post mid timetables
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
@@ -474,7 +474,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 [C202]</t>
+          <t>ELECTIVE_B1 [C104]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -484,17 +484,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 [C202]</t>
+          <t>ELECTIVE_B1 [C104]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>HS161 [C002]</t>
+          <t>MA162 [C304]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 [C404]</t>
         </is>
       </c>
     </row>
@@ -506,27 +506,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MA162 [C205]</t>
+          <t>MA162 [C304]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HS161 [C002]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 [C101]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 [C404]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EC161 [C304]</t>
+          <t>MA161 [C002]</t>
         </is>
       </c>
     </row>
@@ -570,27 +570,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DS161 [C202]</t>
+          <t>HS161 [C101]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA161 [C104]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA162 [C205]</t>
+          <t>DS161 [C002]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>DS161 [C202]</t>
+          <t>MA161 [C002]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L408]</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -622,7 +622,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L408]</t>
+          <t>Free</t>
         </is>
       </c>
     </row>
@@ -639,12 +639,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>EC161 [C304]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 (Lab) [L408]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MA161 [C104]</t>
+          <t>DS161 [C002]</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 (Lab) [L408]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -744,22 +744,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 [C004]</t>
+          <t>ELECTIVE_B1 [C002]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>DS161 [C302]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1 [C004]</t>
+          <t>ELECTIVE_B1 [C002]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>DS161 [C304]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -776,27 +776,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MA162 [C404]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA161 [C004]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>EC161 [C402]</t>
+          <t>DS161 [C302]</t>
         </is>
       </c>
     </row>
@@ -840,27 +840,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>HS161 [C205]</t>
+          <t>MA162 [C401]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HS161 [C205]</t>
+          <t>EC161 (Lab) [L408]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>MA161 [C303]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>EC161 [C304]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>HS161 [C201]</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>EC161 (Lab) [L408]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -904,27 +904,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MA161 [C303]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>MA162 [C401]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DS161 [C304]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L408]</t>
+          <t>HS161 [C201]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>MA162 [C404]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
     </row>
@@ -951,7 +951,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>EC161 (Lab) [L408]</t>
+          <t>Free</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C104</t>
         </is>
       </c>
     </row>
@@ -1116,29 +1116,29 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C304</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>**DS161**</t>
+          <t>**HS161**</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Introduction to DATA science and artificial intelligence</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Rajesh N S</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-0-0-3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1158,34 +1158,34 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C101</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>**HS161**</t>
+          <t>**DS161**</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>Introduction to DATA science and artificial intelligence</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Rajesh N S</t>
+          <t>Girish Revadigar</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3-0-0-0-3</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Partial</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1217,17 +1217,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>**MA161**</t>
+          <t>**EC161**</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Prakash Pawar</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1257,24 +1257,24 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>C404, L408</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>**EC161**</t>
+          <t>**MA161**</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prakash Pawar</t>
+          <t>Ramesh Athe</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>C304, L408</t>
+          <t>C002</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>⚠️ 4 issues</t>
+          <t>[WARN] 4 issues</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1464,7 +1464,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C002</t>
         </is>
       </c>
     </row>
@@ -1511,29 +1511,29 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>C404</t>
+          <t>C401</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>**HS161**</t>
+          <t>**DS161**</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>Introduction to DATA science and artificial intelligence</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rajesh N S</t>
+          <t>Girish Revadigar</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3-0-0-0-3</t>
+          <t>2-0-0-0-2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1553,29 +1553,29 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Partial</t>
+          <t>Complete</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C302</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>**MA161**</t>
+          <t>**EC161**</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ramesh Athe</t>
+          <t>Prakash Pawar</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1590,7 +1590,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0/0</t>
+          <t>2/1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1605,29 +1605,29 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>L408, C003</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>**DS161**</t>
+          <t>**MA161**</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Introduction to DATA science and artificial intelligence</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Girish Revadigar</t>
+          <t>Ramesh Athe</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2-0-0-0-2</t>
+          <t>3-0-2-0-2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1647,34 +1647,34 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C004</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>**EC161**</t>
+          <t>**HS161**</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Prakash Pawar</t>
+          <t>Rajesh N S</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3-0-2-0-2</t>
+          <t>3-0-0-0-3</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2/1</t>
+          <t>0/0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>C402, C304, L408</t>
+          <t>C201</t>
         </is>
       </c>
     </row>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>⚠️ 4 issues</t>
+          <t>[WARN] 4 issues</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1761,7 +1761,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1838,41 +1838,41 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>A, B</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>DS161, MA161, ELECTIVE_B1</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>1.2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1905,17 +1905,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>240</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -1948,7 +1948,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1967,7 +1967,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -1975,23 +1975,23 @@
         </is>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>ELECTIVE_B1, DS161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2010,31 +2010,31 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>MA162, HS161</t>
+          <t>ELECTIVE_B1</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>C201</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -2077,7 +2077,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2096,31 +2096,31 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>B</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>DS161, EC161</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C402</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2139,11 +2139,11 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -2151,19 +2151,19 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>0.2</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C404</t>
+          <t>C401</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>96</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2206,12 +2206,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C404</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>classroom without projector</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2221,15 +2221,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Computers</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>A, B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -2237,10 +2237,53 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>L408</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>classroom without projector</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>A, B</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
           <t>EC161 (Lab)</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>0.8</t>
         </is>
@@ -2355,22 +2398,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>✅ FULLY COMPLIANT</t>
+          <t>[OK] FULLY COMPLIANT</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -2412,22 +2455,22 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>⚠️ PARTIAL</t>
+          <t>[WARN] PARTIAL</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -2469,22 +2512,22 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>⚠️ PARTIAL</t>
+          <t>[WARN] PARTIAL</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -2526,22 +2569,22 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>⚠️ PARTIAL</t>
+          <t>[WARN] PARTIAL</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -2583,22 +2626,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>[FAIL]</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>⚠️ PARTIAL</t>
+          <t>[WARN] PARTIAL</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -2640,22 +2683,22 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>✅</t>
+          <t>[OK]</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>✅ FULLY COMPLIANT</t>
+          <t>[OK] FULLY COMPLIANT</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -2738,7 +2781,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-12-03 12:04</t>
+          <t>2025-12-12 16:58</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2822,12 +2865,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>10/35</t>
+          <t>11/35</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Utilization: 28.6%</t>
+          <t>Utilization: 31.4%</t>
         </is>
       </c>
     </row>
@@ -2866,7 +2909,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>⚠️ NEEDS REVIEW</t>
+          <t>[WARN] NEEDS REVIEW</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">

</xml_diff>

<commit_message>
Stricter separation of departement specific pre mid and post mid courses
</commit_message>
<xml_diff>
--- a/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
+++ b/backend/output_timetables/sem1_CSE_timetable_baskets.xlsx
@@ -526,7 +526,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>CS161 [C202]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -612,7 +612,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CS161 (Lab) [L207]</t>
+          <t>CS161 (Lab) [L106]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -671,17 +671,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MA162 [C004]</t>
+          <t>MA162 [C003]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EC161 [C004]</t>
+          <t>EC161 [C003]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CS161 [C004]</t>
+          <t>CS161 [C202]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MA161 [C001]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CS161 [C001]</t>
+          <t>CS161 [C203]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -882,17 +882,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MA161 [C001]</t>
+          <t>MA161 [C003]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DS161 [C001]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -946,12 +946,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DS161 [C001]</t>
+          <t>DS161 [C003]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>MA162 [C001]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1010,17 +1010,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>MA162 [C001]</t>
+          <t>MA162 [C004]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EC161 [C001]</t>
+          <t>EC161 [C004]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>CS161 [C001]</t>
+          <t>CS161 [C203]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2747,16 +2747,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>37.5</v>
+        <v>0</v>
       </c>
       <c r="H2" t="inlineStr"/>
     </row>
@@ -2811,16 +2811,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2845,16 +2845,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>37.5</v>
+        <v>30</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -3049,16 +3049,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>6.25</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -3151,16 +3151,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -3185,16 +3185,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -3321,16 +3321,16 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -3389,16 +3389,16 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E21" t="n">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -4206,17 +4206,17 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J4" t="b">
@@ -4230,7 +4230,7 @@
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -4422,17 +4422,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J7" t="b">
@@ -4446,7 +4446,7 @@
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
@@ -4494,17 +4494,17 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J8" t="b">
@@ -4518,7 +4518,7 @@
       <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -4566,17 +4566,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J9" t="b">
@@ -4590,7 +4590,7 @@
       <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -4782,17 +4782,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J12" t="b">
@@ -4806,7 +4806,7 @@
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -4854,17 +4854,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J13" t="b">
@@ -4878,7 +4878,7 @@
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -5022,7 +5022,7 @@
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="inlineStr">
         <is>
-          <t>L207</t>
+          <t>L106</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -5094,7 +5094,7 @@
       <c r="L16" t="inlineStr"/>
       <c r="M16" t="inlineStr">
         <is>
-          <t>L207</t>
+          <t>L106</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -5214,12 +5214,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
@@ -5295,7 +5295,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -5371,7 +5371,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>L403</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -5447,7 +5447,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -5470,7 +5470,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -5523,12 +5523,12 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J22" t="b">
@@ -5546,7 +5546,7 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -5622,7 +5622,7 @@
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -5670,17 +5670,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J24" t="b">
@@ -5698,7 +5698,7 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>L402</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
@@ -5827,7 +5827,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -5850,7 +5850,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>L407</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -5898,17 +5898,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J27" t="b">
@@ -5926,7 +5926,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
@@ -5974,12 +5974,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -6002,7 +6002,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
@@ -6131,7 +6131,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>L403</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
@@ -6207,7 +6207,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -6283,12 +6283,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J32" t="b">
@@ -6306,7 +6306,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -6382,7 +6382,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
@@ -6430,17 +6430,17 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J34" t="b">
@@ -6458,7 +6458,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
@@ -6534,7 +6534,7 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>L402</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -6610,7 +6610,7 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>L407</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
@@ -6658,17 +6658,17 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J37" t="b">
@@ -6686,7 +6686,7 @@
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
@@ -6734,12 +6734,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>135</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>C302</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
@@ -6815,7 +6815,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -6838,7 +6838,7 @@
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>C303</t>
+          <t>L402</t>
         </is>
       </c>
       <c r="N39" t="inlineStr">
@@ -6891,7 +6891,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>C304</t>
+          <t>L403</t>
         </is>
       </c>
       <c r="N40" t="inlineStr">
@@ -6967,7 +6967,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
@@ -6990,7 +6990,7 @@
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>L408</t>
+          <t>C305</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
@@ -7043,12 +7043,12 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J42" t="b">
@@ -7066,7 +7066,7 @@
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>L406</t>
+          <t>C302</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
@@ -7119,7 +7119,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -7142,7 +7142,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>C305</t>
+          <t>L404</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -7190,17 +7190,17 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>135</t>
+          <t>80</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Projector</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J44" t="b">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>C003</t>
+          <t>L405</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
@@ -7294,7 +7294,7 @@
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>L402</t>
+          <t>L406</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -7347,7 +7347,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -7370,7 +7370,7 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>L407</t>
+          <t>C303</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
@@ -7418,17 +7418,17 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Auditorium</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>240</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Audio/Video System</t>
+          <t>TV</t>
         </is>
       </c>
       <c r="J47" t="b">
@@ -7446,7 +7446,7 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>C304</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
@@ -7499,10 +7499,14 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr"/>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J48" t="b">
         <v>0</v>
       </c>
@@ -7514,7 +7518,7 @@
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
@@ -7567,10 +7571,14 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr"/>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J49" t="b">
         <v>0</v>
       </c>
@@ -7582,7 +7590,7 @@
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
@@ -7630,15 +7638,19 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J50" t="b">
         <v>0</v>
       </c>
@@ -7650,7 +7662,7 @@
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
@@ -7703,10 +7715,14 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr"/>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J51" t="b">
         <v>0</v>
       </c>
@@ -7718,7 +7734,7 @@
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N51" t="inlineStr">
@@ -7771,10 +7787,14 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr"/>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
       <c r="J52" t="b">
         <v>0</v>
       </c>
@@ -7786,7 +7806,7 @@
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C003</t>
         </is>
       </c>
       <c r="N52" t="inlineStr">
@@ -7834,15 +7854,19 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J53" t="b">
         <v>0</v>
       </c>
@@ -7854,7 +7878,7 @@
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N53" t="inlineStr">
@@ -7902,15 +7926,19 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J54" t="b">
         <v>0</v>
       </c>
@@ -7922,7 +7950,7 @@
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
@@ -7970,15 +7998,19 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J55" t="b">
         <v>0</v>
       </c>
@@ -7990,7 +8022,7 @@
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N55" t="inlineStr">
@@ -8182,15 +8214,19 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
       <c r="J58" t="b">
         <v>0</v>
       </c>
@@ -8202,7 +8238,7 @@
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N58" t="inlineStr">
@@ -8250,15 +8286,19 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>classroom</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr"/>
+          <t>96</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
       <c r="J59" t="b">
         <v>0</v>
       </c>
@@ -8270,7 +8310,7 @@
       <c r="L59" t="inlineStr"/>
       <c r="M59" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N59" t="inlineStr">
@@ -8606,15 +8646,19 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J64" t="b">
         <v>0</v>
       </c>
@@ -8630,7 +8674,7 @@
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
@@ -8686,11 +8730,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
+      <c r="I65" t="inlineStr"/>
       <c r="J65" t="b">
         <v>0</v>
       </c>
@@ -8706,7 +8746,7 @@
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C001</t>
         </is>
       </c>
       <c r="N65" t="inlineStr">
@@ -8754,12 +8794,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>120</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -8782,7 +8822,7 @@
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="N66" t="inlineStr">
@@ -8858,7 +8898,7 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>C102</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N67" t="inlineStr">
@@ -8934,7 +8974,7 @@
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N68" t="inlineStr">
@@ -9010,7 +9050,7 @@
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
@@ -9068,7 +9108,7 @@
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J70" t="b">
@@ -9086,7 +9126,7 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N70" t="inlineStr">
@@ -9162,7 +9202,7 @@
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N71" t="inlineStr">
@@ -9238,7 +9278,7 @@
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N72" t="inlineStr">
@@ -9291,7 +9331,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -9314,7 +9354,7 @@
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>L403</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N73" t="inlineStr">
@@ -9362,15 +9402,19 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J74" t="b">
         <v>0</v>
       </c>
@@ -9386,7 +9430,7 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N74" t="inlineStr">
@@ -9442,11 +9486,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
+      <c r="I75" t="inlineStr"/>
       <c r="J75" t="b">
         <v>0</v>
       </c>
@@ -9462,7 +9502,7 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C001</t>
         </is>
       </c>
       <c r="N75" t="inlineStr">
@@ -9510,12 +9550,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>120</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -9538,7 +9578,7 @@
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="N76" t="inlineStr">
@@ -9614,7 +9654,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>C102</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N77" t="inlineStr">
@@ -9690,7 +9730,7 @@
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N78" t="inlineStr">
@@ -9766,7 +9806,7 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
@@ -9824,7 +9864,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J80" t="b">
@@ -9842,7 +9882,7 @@
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
@@ -9918,7 +9958,7 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -9994,7 +10034,7 @@
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N82" t="inlineStr">
@@ -10047,7 +10087,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -10070,7 +10110,7 @@
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>L403</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N83" t="inlineStr">
@@ -10118,15 +10158,19 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>large classroom</t>
+          <t>Auditorium</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>120</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr"/>
+          <t>240</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>Audio/Video System</t>
+        </is>
+      </c>
       <c r="J84" t="b">
         <v>0</v>
       </c>
@@ -10142,7 +10186,7 @@
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>C001</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="N84" t="inlineStr">
@@ -10198,11 +10242,7 @@
           <t>120</t>
         </is>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>Projector</t>
-        </is>
-      </c>
+      <c r="I85" t="inlineStr"/>
       <c r="J85" t="b">
         <v>0</v>
       </c>
@@ -10218,7 +10258,7 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>C002</t>
+          <t>C001</t>
         </is>
       </c>
       <c r="N85" t="inlineStr">
@@ -10266,12 +10306,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>classroom</t>
+          <t>large classroom</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>120</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -10294,7 +10334,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>C101</t>
+          <t>C002</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
@@ -10370,7 +10410,7 @@
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>C102</t>
+          <t>C101</t>
         </is>
       </c>
       <c r="N87" t="inlineStr">
@@ -10446,7 +10486,7 @@
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>C104</t>
+          <t>C102</t>
         </is>
       </c>
       <c r="N88" t="inlineStr">
@@ -10522,7 +10562,7 @@
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>C202</t>
+          <t>C104</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
@@ -10580,7 +10620,7 @@
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>TV</t>
+          <t>Projector</t>
         </is>
       </c>
       <c r="J90" t="b">
@@ -10598,7 +10638,7 @@
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>C203</t>
+          <t>C202</t>
         </is>
       </c>
       <c r="N90" t="inlineStr">
@@ -10674,7 +10714,7 @@
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>C204</t>
+          <t>C203</t>
         </is>
       </c>
       <c r="N91" t="inlineStr">
@@ -10750,7 +10790,7 @@
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>C205</t>
+          <t>C204</t>
         </is>
       </c>
       <c r="N92" t="inlineStr">
@@ -10803,7 +10843,7 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>80</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
@@ -10826,7 +10866,7 @@
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>L403</t>
+          <t>C205</t>
         </is>
       </c>
       <c r="N93" t="inlineStr">
@@ -10892,7 +10932,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C001, C302</t>
+          <t>C003, C004</t>
         </is>
       </c>
     </row>
@@ -10909,7 +10949,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C002, C303</t>
+          <t>C001, L402</t>
         </is>
       </c>
     </row>
@@ -10926,7 +10966,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C101, C304</t>
+          <t>C002, L403</t>
         </is>
       </c>
     </row>
@@ -10943,7 +10983,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>C102, L408</t>
+          <t>C101, C305</t>
         </is>
       </c>
     </row>
@@ -10960,7 +11000,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C104, L406</t>
+          <t>C102, C302</t>
         </is>
       </c>
     </row>
@@ -10977,7 +11017,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>C202, C305</t>
+          <t>C104, L404</t>
         </is>
       </c>
     </row>
@@ -10994,7 +11034,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C003, C203</t>
+          <t>C202, L405</t>
         </is>
       </c>
     </row>
@@ -11011,7 +11051,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>C204, L402</t>
+          <t>C203, L406</t>
         </is>
       </c>
     </row>
@@ -11028,7 +11068,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>C205, L407</t>
+          <t>C204, C303</t>
         </is>
       </c>
     </row>
@@ -11045,7 +11085,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>C004, L403</t>
+          <t>C205, C304</t>
         </is>
       </c>
     </row>

</xml_diff>